<commit_message>
Completed with 4337 patients
</commit_message>
<xml_diff>
--- a/completed_countries.xlsx
+++ b/completed_countries.xlsx
@@ -470,7 +470,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -511,7 +511,9 @@
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="5">
+        <v>3100</v>
+      </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
@@ -565,7 +567,7 @@
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="8"/>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="6" t="s">
@@ -573,7 +575,7 @@
       </c>
       <c r="B15" s="7">
         <f>SUM(B3:B14)</f>
-        <v>1244</v>
+        <v>4344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed with 7714 patients.
</commit_message>
<xml_diff>
--- a/completed_countries.xlsx
+++ b/completed_countries.xlsx
@@ -100,7 +100,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,12 +110,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -147,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -168,9 +162,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -470,7 +461,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -512,7 +503,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="5">
-        <v>3100</v>
+        <v>3091</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -567,7 +558,9 @@
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="5">
+        <v>3379</v>
+      </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="6" t="s">
@@ -575,7 +568,7 @@
       </c>
       <c r="B15" s="7">
         <f>SUM(B3:B14)</f>
-        <v>4344</v>
+        <v>7714</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed with 8240 patients.
</commit_message>
<xml_diff>
--- a/completed_countries.xlsx
+++ b/completed_countries.xlsx
@@ -100,7 +100,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,6 +110,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -141,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -162,6 +168,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -461,7 +470,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -528,7 +537,7 @@
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="8"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="4" t="s">

</xml_diff>

<commit_message>
Completed with 10037 patients.
</commit_message>
<xml_diff>
--- a/completed_countries.xlsx
+++ b/completed_countries.xlsx
@@ -1,17 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144E3B3D-8879-403D-8D50-B080E08C6443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -69,8 +83,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -170,7 +184,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -179,13 +196,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -223,7 +248,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -257,6 +282,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -291,9 +317,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -466,20 +493,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -487,13 +514,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -501,13 +528,13 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3"/>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -515,55 +542,57 @@
         <v>3091</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="8"/>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="B9" s="8">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
@@ -571,13 +600,13 @@
         <v>3379</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="7">
         <f>SUM(B3:B14)</f>
-        <v>7714</v>
+        <v>9218</v>
       </c>
     </row>
   </sheetData>
@@ -587,24 +616,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed with 11982 patients.
</commit_message>
<xml_diff>
--- a/completed_countries.xlsx
+++ b/completed_countries.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144E3B3D-8879-403D-8D50-B080E08C6443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7615C255-9910-4825-95C7-6BC750118495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,7 +114,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,12 +124,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -161,15 +155,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -185,9 +176,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -497,7 +485,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,106 +495,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="4">
+        <v>345</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>1244</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="4">
+        <v>67</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>3091</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="4">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="9"/>
+      <c r="B7" s="4">
+        <v>974</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="4">
+        <v>37</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>1504</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="4">
+        <v>756</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="4">
+        <v>465</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="4">
+        <v>101</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>3379</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="7">
-        <f>SUM(B3:B14)</f>
-        <v>9218</v>
+      <c r="B15" s="6">
+        <f>SUM(B2:B14)</f>
+        <v>11980</v>
       </c>
     </row>
   </sheetData>

</xml_diff>